<commit_message>
Working on activate account
</commit_message>
<xml_diff>
--- a/AlumniHub.xlsx
+++ b/AlumniHub.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laxma\OneDrive\Desktop\AlumniHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA01F51A-D69A-450A-B828-4A07B2E14333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{480C4DD8-1B76-4879-9DA1-A2625CAD2485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,13 +64,13 @@
     <t>Mangesh vispute</t>
   </si>
   <si>
-    <t>mangesh2004vispute@gmail.com</t>
-  </si>
-  <si>
     <t>Year_joined</t>
   </si>
   <si>
     <t>graduation_year</t>
+  </si>
+  <si>
+    <t>mangesh2003vispute@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -411,7 +411,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -446,10 +446,10 @@
         <v>7</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>0</v>
@@ -466,7 +466,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D2">
         <v>9307168315</v>

</xml_diff>

<commit_message>
edit profile icon is done
</commit_message>
<xml_diff>
--- a/AlumniHub.xlsx
+++ b/AlumniHub.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laxma\OneDrive\Desktop\AlumniHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB331D07-E62B-4BB3-A415-952F65DC3B12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE844F3-DFE9-4608-8C71-9C12F2D2786C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -414,7 +414,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -485,7 +485,7 @@
       <c r="J2">
         <v>2025</v>
       </c>
-      <c r="K2" t="b">
+      <c r="L2" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
workflow improved for activate email
</commit_message>
<xml_diff>
--- a/AlumniHub.xlsx
+++ b/AlumniHub.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laxma\OneDrive\Desktop\AlumniHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E53B8167-1AEB-44D9-A225-09F4CF83B521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D30142F-EC02-46BE-AB03-5E0FFC97A9D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>is_alumni</t>
   </si>
@@ -74,18 +74,6 @@
   </si>
   <si>
     <t>graduation_month</t>
-  </si>
-  <si>
-    <t>Chetan Sonar</t>
-  </si>
-  <si>
-    <t>chetansonar2003@gmail.com</t>
-  </si>
-  <si>
-    <t>Rohan sapkale</t>
-  </si>
-  <si>
-    <t>99beastrohan@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -423,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -497,67 +485,13 @@
       <c r="J2">
         <v>2025</v>
       </c>
-      <c r="L2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3">
-        <v>7498530829</v>
-      </c>
-      <c r="H3">
-        <v>2021</v>
-      </c>
-      <c r="I3">
-        <v>5</v>
-      </c>
-      <c r="J3">
-        <v>2025</v>
-      </c>
-      <c r="L3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4">
-        <v>9511672132</v>
-      </c>
-      <c r="H4">
-        <v>2021</v>
-      </c>
-      <c r="I4">
-        <v>5</v>
-      </c>
-      <c r="J4">
-        <v>2025</v>
-      </c>
-      <c r="L4" t="b">
+      <c r="K2" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{44BC32FF-65E5-4404-AF1C-6B8ED765BD6C}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{56D7C03E-E17D-4BBE-AA4D-F85F61E2B548}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{50E8D320-BA0B-41E6-8497-D2DCC58CF5E5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>